<commit_message>
Database Schema minor change
</commit_message>
<xml_diff>
--- a/Project/Database/Database Schema.xlsx
+++ b/Project/Database/Database Schema.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
   <si>
     <t>Column</t>
   </si>
@@ -52,9 +52,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>number/int</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>Varchar</t>
   </si>
   <si>
-    <t>Number/Int</t>
-  </si>
-  <si>
     <t>Book</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Service Provider</t>
-  </si>
-  <si>
     <t>Total Payment</t>
   </si>
   <si>
@@ -142,24 +133,15 @@
     <t>Street Name</t>
   </si>
   <si>
-    <t>House Number</t>
-  </si>
-  <si>
     <t>Postal Code</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Rate</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -224,6 +206,33 @@
   </si>
   <si>
     <t>Foreign Key(Block)</t>
+  </si>
+  <si>
+    <t>Not null,unique</t>
+  </si>
+  <si>
+    <t>not null</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>House number</t>
+  </si>
+  <si>
+    <t>Favourite Pro ID</t>
+  </si>
+  <si>
+    <t>Block Pro ID</t>
+  </si>
+  <si>
+    <t>Provider ID</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>not null,unique</t>
   </si>
 </sst>
 </file>
@@ -275,13 +284,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +588,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,20 +599,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -612,10 +621,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -625,13 +634,19 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -641,6 +656,9 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -649,21 +667,24 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -673,38 +694,41 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +745,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -733,7 +757,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -744,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -752,96 +776,111 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -851,10 +890,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -865,11 +904,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -879,18 +918,18 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -898,72 +937,81 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -971,31 +1019,23 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1022,11 +1062,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -1036,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1044,32 +1084,32 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1125,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C1:C1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1096,11 +1136,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -1110,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1118,61 +1158,70 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1180,6 +1229,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1188,7 +1238,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1199,11 +1249,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -1213,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1221,32 +1271,32 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1262,7 +1312,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1273,11 +1323,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -1287,42 +1337,51 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>